<commit_message>
working on yadisc function
</commit_message>
<xml_diff>
--- a/shippers/xiaomi.xlsx
+++ b/shippers/xiaomi.xlsx
@@ -10,8 +10,8 @@
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$A$1:$C$324</definedName>
-    <definedName name="Z_5BF74F22_93CB_493F_8338_9D1106536A76_.wvu.FilterData" localSheetId="0" hidden="1">Лист1!$A$1:$C$323</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$A$1:$C$309</definedName>
+    <definedName name="Z_5BF74F22_93CB_493F_8338_9D1106536A76_.wvu.FilterData" localSheetId="0" hidden="1">Лист1!$A$1:$C$308</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <customWorkbookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="311">
   <si>
     <t>Наименование</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Xiaomi Redmi 9C 128Gb 4Gb (Twilight Blue) EU</t>
   </si>
   <si>
-    <t>Xiaomi Redmi Note 10 Pro 256Gb 8Gb (Onyx Gray) EU</t>
-  </si>
-  <si>
     <t>Xiaomi Redmi Note 11 128GB 4Gb (Twilight blue) RU</t>
   </si>
   <si>
@@ -122,9 +119,6 @@
     <t>Xiaomi Poco M5 128Gb 6Gb (Green) EU</t>
   </si>
   <si>
-    <t>Xiaomi Redmi 10 128Gb 6Gb (Gray) EU</t>
-  </si>
-  <si>
     <t>Xiaomi Redmi 10A 64Gb 4Gb (Charcoal Black) CN</t>
   </si>
   <si>
@@ -341,9 +335,6 @@
     <t>Xiaomi Poco X5 256Gb 8Gb (Green) RU</t>
   </si>
   <si>
-    <t>Xiaomi Redmi 10 (2022) 128gb 4gb (Carbon Grey) EU</t>
-  </si>
-  <si>
     <t>Xiaomi Redmi 10 (2022) 128gb 6gb (Pebble White) EU</t>
   </si>
   <si>
@@ -416,18 +407,12 @@
     <t>Xiaomi Redmi Pad Wi-Fi 4Gb 128Gb (Graphite Gray) RU</t>
   </si>
   <si>
-    <t>Xiaomi Redmi Pad Wi-Fi 4Gb 128Gb (Mint Green) RU</t>
-  </si>
-  <si>
     <t>Xiaomi Redmi Pad Wi-Fi 4Gb 128Gb (Moonlight Silver) RU</t>
   </si>
   <si>
     <t>Xiaomi Redmi Note 10 Pro 128Gb 8Gb (Onyx Gray) RU</t>
   </si>
   <si>
-    <t>Xiaomi Redmi Note 10 Pro 256Gb 8Gb (Glacier Blue) EU</t>
-  </si>
-  <si>
     <t>Xiaomi Redmi Note 10 Pro 64Gb 6Gb (Glacier Blue) EU</t>
   </si>
   <si>
@@ -467,70 +452,463 @@
     <t>Xiaomi Redmi Note 11 Pro Plus 5G 256Gb 8Gb (Graphite Gray) EU</t>
   </si>
   <si>
+    <t>Xiaomi 13 Lite 256Gb 8Gb (Blue) RU</t>
+  </si>
+  <si>
+    <t>Xiaomi Poco F4 128Gb 6Gb (Moonlight Silver) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Poco F4 128Gb 6Gb (Nebula Green) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Pad Wi-Fi 6Gb 128Gb (Graphite Gray) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Pad Wi-Fi 6Gb 128Gb (Moonlight Silver) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi 11T Pro 256Gb 8Gb (Meteorite Gray) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi 12 Lite 5G 128Gb 8Gb (Lite Green) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi 12T 256Gb 8Gb (Blue) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi 12X 128Gb 8Gb (Gray) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi 12c 64GB 3Gb (Violet) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi 13 256Gb 8GB (Black) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi 13 256Gb 8GB (Green) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi 13 pro 256Gb 12Gb (Ceramic Black) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi 13 pro 256Gb 12Gb (Ceramic White) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Poco F4 256Gb 8Gb (Night Black) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Poco M5 64Gb 4Gb (Yellow) EU NFC</t>
+  </si>
+  <si>
+    <t>Xiaomi Poco X5 128GB 6Gb (Blue) RU</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi 10 (2022) 128gb 4gb (Sea Blue) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi 10 (2022) 128gb 4gb (Sea Blue) RU</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi 10A 32Gb 2Gb (Sea Blue) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi 10c 128Gb 4Gb (Graphite Gray) EU with NFC</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi 10c 128Gb 4Gb (Mint Green) EU with NFC</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi 10c 128Gb 4Gb (Ocean Blue) EU with NFC</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi 10c 64Gb 3Gb (Graphite Gray) EU with NFC</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi 10c 64Gb 4Gb (Graphite Gray) EU with NFC</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi 9A 32Gb 2Gb (Granite Gray) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi 9A 32Gb 2Gb (Peacook Green) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi 9A 32Gb 2Gb (Sky Blue) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi 9C 32Gb 2Gb (Sunrise Orange) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 11 128GB 4Gb (Mysterious Black) CN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xiaomi Redmi Note 11 Pro Plus 5G 128Gb 8Gb (Forest Green) </t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 11E Pro 128Gb 8Gb (Atlantic Blue) CN</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 11E Pro 128Gb 8Gb (Graphite Gray) CN</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 11E Pro 128Gb 8Gb (Polar White) CN</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 11E Pro 256Gb 8Gb (Graphite Gray) CN</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 11E Pro 256Gb 8Gb (Polar White) CN</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 11S 128Gb 6Gb (Graphite Gray) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 11S 128Gb 6Gb (Twilight Blue) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Pad Wi-Fi 128Gb (Moonlight Silver) CN</t>
+  </si>
+  <si>
+    <t>Xiaomi 12 Lite 5G 128Gb 8Gb (Black) RU</t>
+  </si>
+  <si>
+    <t>Xiaomi 12c 64GB 3Gb (Mint) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi 13 Lite 256Gb 8Gb (Pink) RU</t>
+  </si>
+  <si>
+    <t>Xiaomi Mix Fold 2 12Gb 256Gb (Black) CN</t>
+  </si>
+  <si>
+    <t>Xiaomi Mix Fold 2 12Gb 512Gb (Black) CN</t>
+  </si>
+  <si>
+    <t>Xiaomi Poco F4 128Gb 8Gb (Moonlight Silver) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Poco M5 128Gb 6Gb (Black) EU NFC</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi 10 128Gb 6Gb (Blue) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi 10A 128Gb 4Gb (Graphite Grey) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi 10c 64Gb 3Gb (Mint Green) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi 10c 64Gb 3Gb (Ocean Blue) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 10 JE 64Gb 4Gb (White) JP</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 10 Pro 128Gb 8Gb (Glacier Blue) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 11 Pro 5G 64Gb 6GB (Graphite Gray) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 11 Pro Plus 5G 128Gb 8Gb (Graphite Gray) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 12 128GB 6GB (Blue) CN</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 12 128GB 6GB (White) CN</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 12 Pro 256GB 8GB (Black) CN</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 12 Pro+ 256GB 12GB (Blue) CN</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 12 Pro+ 256GB 8GB (Black) CN</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 12 Pro+ 256GB 8GB (Blue) CN</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 12 Pro+ 256GB 8GB (White) CN</t>
+  </si>
+  <si>
+    <t>Xiaomi 12 256Gb 12GB (Blue) RU</t>
+  </si>
+  <si>
+    <t>Xiaomi 12T Pro 256Gb 8Gb (Black) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi 12c 128Gb 6GB (Gray) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi 13 Lite 256Gb 8Gb (Black) RU</t>
+  </si>
+  <si>
+    <t>Xiaomi Poco X5 Pro 256GB 8GB (Blue) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 12 128GB 4Gb (Black) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 12 Pro 256GB 8GB (Violet) CN</t>
+  </si>
+  <si>
+    <t>Xiaomi 12X 128Gb 8Gb (Blue) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi 12X 256Gb 8Gb (Blue) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi 12X 256Gb 8Gb (Gray) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi 12c 128Gb 6GB (Mint) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi 13 Lite 256Gb 8Gb (Black) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Poco C40 64Gb 4Gb (Poco Yellow) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Poco M5 64Gb 4Gb (Black) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Poco X5 128GB 6Gb (Black) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi 10 128Gb 4Gb (White) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 11 Pro 128Gb 8Gb (Graphite Gray) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 11 Pro 128Gb 8Gb (Polar White) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi 11T 128Gb 8Gb (Celestial Blue) RU</t>
+  </si>
+  <si>
+    <t>Xiaomi 11T 128Gb 8Gb (Meteorite Gray) RU</t>
+  </si>
+  <si>
+    <t>Xiaomi 12c 64GB 4Gb (Blue) EU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xiaomi 13 Lite 256Gb 8Gb (Black) </t>
+  </si>
+  <si>
+    <t>Xiaomi Mi 10T 5G 128Gb 8Gb (Cosmic Black) RU</t>
+  </si>
+  <si>
+    <t>Xiaomi Mi 10T 5G 128Gb 8Gb (Lunar Silver) RU</t>
+  </si>
+  <si>
+    <t>Xiaomi Pad 5 Wi-Fi 128Gb (Cosmic Gray) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Pad 5 Wi-Fi 256Gb (Cosmic Gray) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Poco M4 Pro 5G 64Gb 4Gb (Cool Blue) RU</t>
+  </si>
+  <si>
+    <t>Xiaomi Poco M4 Pro 5G 64Gb 4Gb (Poco Yellow) RU</t>
+  </si>
+  <si>
+    <t>Xiaomi Poco M5s 128Gb 4Gb (Blue) RU</t>
+  </si>
+  <si>
+    <t>Xiaomi Poco M5s 128Gb 4Gb (Gray) RU</t>
+  </si>
+  <si>
+    <t>Xiaomi Poco M5s 128Gb 4Gb (White) RU</t>
+  </si>
+  <si>
+    <t>Xiaomi Poco M5s 128Gb 4Gb (Yellow) RU</t>
+  </si>
+  <si>
+    <t>Xiaomi Poco X4 Pro 5G 128Gb 6Gb (Laser Black) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Poco X5 Pro 128GB 6GB (Yellow) RU</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 10 5G 128Gb 4Gb (Aurora Green) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 10S 128Gb 8Gb (Ocean Blue) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 11 128GB 4Gb (Starlight blue) CN</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 11 Pro 128Gb 6Gb (Atlantic Blue) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 11 Pro 5G 128Gb 6GB (Graphite Gray) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 11 Pro 5G 128Gb 8GB (Graphite Gray) RU</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 11S 128Gb 8Gb (Pearl White) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 11 Pro 128Gb 6Gb (Polar White) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 11 Pro 128Gb 6Gb (Star Blue) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 11 Pro 128Gb 8Gb (Atlantic Blue) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi 12T 128Gb 8Gb (Blue) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi 12T Pro 256Gb 8Gb (Blue) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi 13 Lite 128Gb 8Gb (Black) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Poco F4 GT 128Gb 8Gb (Knight Silver) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Poco F4 GT 256Gb 12Gb (Stealth Black) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Poco X5 128GB 6Gb (Black) RU</t>
+  </si>
+  <si>
+    <t>Xiaomi Poco X5 256Gb 8Gb (Black) RU</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 12 Pro 256GB 8GB (White) CN</t>
+  </si>
+  <si>
+    <t>Xiaomi 12 256Gb 12GB (Gray) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Black Shark 5 Pro 256Gb 16Gb (Black) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Black Shark 5 Pro 256Gb 16Gb (White) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Pad 5 Wi-Fi 128Gb (Pearl White) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Pad 5 Wi-Fi 256Gb (Pearl White) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi 10 (2022) 128gb 6gb (Carbon Grey) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi 10 64Gb 4Gb (White) EU with NFC</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 11 Pro 128Gb 8Gb (Graphite Gray) RU</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Pad Wi-Fi 4Gb 128Gb (Mint Green) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Pad Wi-Fi 6Gb 128Gb (Mint Green) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi 11T Pro 128Gb 8Gb (Celestial Blue) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi 12T Pro 256Gb 12Gb (Blue) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi 12c 128Gb 4Gb (Blue) RU</t>
+  </si>
+  <si>
+    <t>Xiaomi 12c 128Gb 4Gb (Gray) RU</t>
+  </si>
+  <si>
+    <t>Xiaomi 12c 128Gb 4Gb (Violet) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi 12c 128Gb 4Gb (Violet) RU</t>
+  </si>
+  <si>
+    <t>Xiaomi 12c 64GB 3Gb (Gray) RU</t>
+  </si>
+  <si>
+    <t>Xiaomi 12c 64GB 3Gb (Violet) RU</t>
+  </si>
+  <si>
+    <t>Xiaomi Pad 5 Wi-Fi 128Gb (Pearl White) CN</t>
+  </si>
+  <si>
+    <t>Xiaomi Poco M5s 128Gb 4Gb (Gray) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Poco M5s 64Gb 4Gb (Blue) RU</t>
+  </si>
+  <si>
+    <t>Xiaomi Poco M5s 64Gb 4Gb (Gray) RU</t>
+  </si>
+  <si>
+    <t>Xiaomi Poco M5s 64Gb 4Gb (White) RU</t>
+  </si>
+  <si>
+    <t>Xiaomi Poco M5s 64Gb 4Gb (Yellow) RU</t>
+  </si>
+  <si>
+    <t>Xiaomi Poco X4 GT 256Gb 8Gb (Silver) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 10S 128Gb 6Gb (Frost White) RU</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 11 Pro 5G 128Gb 6GB (Polar White) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Poco F3 256Gb 8Gb (Arctic White) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Poco M5 128Gb 6Gb (Black) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Poco X5 Pro 256GB 6GB (Blue) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 10S 128Gb 6Gb (Frost White) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 10S 128Gb 6Gb (Ocean Blue) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 11 128GB 6GB (Graphite Gray) CN</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 11 128GB 6GB (Pearl White) CN</t>
+  </si>
+  <si>
+    <t>Xiaomi 12 Lite 5G 128Gb 6Gb (Black) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi 12 Lite 5G 256Gb 8Gb (Lite Green) EU</t>
+  </si>
+  <si>
     <t>Xiaomi 12 Pro 256GB 12GB (Gray) EU</t>
   </si>
   <si>
-    <t>Xiaomi 13 Lite 256Gb 8Gb (Blue) RU</t>
-  </si>
-  <si>
-    <t>Xiaomi Poco F4 128Gb 6Gb (Moonlight Silver) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Poco F4 128Gb 6Gb (Nebula Green) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi Pad Wi-Fi 6Gb 128Gb (Graphite Gray) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi Pad Wi-Fi 6Gb 128Gb (Moonlight Silver) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi 11T Pro 256Gb 8Gb (Meteorite Gray) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi 12 Lite 5G 128Gb 8Gb (Lite Green) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi 12T 256Gb 8Gb (Blue) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi 12T 256Gb 8Gb (Silver) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi 12X 128Gb 8Gb (Gray) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi 12c 64GB 3Gb (Violet) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi 12c 64GB 4Gb (Mint) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi 13 256Gb 8GB (Black) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi 13 256Gb 8GB (Green) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi 13 pro 256Gb 12Gb (Ceramic Black) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi 13 pro 256Gb 12Gb (Ceramic White) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Poco F4 256Gb 8Gb (Night Black) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Poco M5 64Gb 4Gb (Yellow) EU NFC</t>
-  </si>
-  <si>
-    <t>Xiaomi Poco X5 128GB 6Gb (Blue) RU</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi 10 (2022) 128gb 4gb (Sea Blue) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi 10 (2022) 128gb 4gb (Sea Blue) RU</t>
+    <t>Xiaomi 12T Pro 128Gb 8Gb (Black) RU</t>
+  </si>
+  <si>
+    <t>Xiaomi 12c 64GB 3Gb (Blue) RU</t>
+  </si>
+  <si>
+    <t>Xiaomi Pad 5 Wi-Fi 128Gb (Pearl White) RU</t>
   </si>
   <si>
     <t>Xiaomi Redmi 10 64Gb 4Gb (Blue) RU</t>
@@ -539,133 +917,31 @@
     <t>Xiaomi Redmi 10 64Gb 4Gb (Gray) RU</t>
   </si>
   <si>
-    <t>Xiaomi Redmi 10 64Gb 4Gb (White) RU</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi 10A 32Gb 2Gb (Sea Blue) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi 10c 128Gb 4Gb (Graphite Gray) EU with NFC</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi 10c 128Gb 4Gb (Mint Green) EU with NFC</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi 10c 128Gb 4Gb (Ocean Blue) EU with NFC</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi 10c 64Gb 3Gb (Graphite Gray) EU with NFC</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi 10c 64Gb 4Gb (Graphite Gray) EU with NFC</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi 9A 32Gb 2Gb (Granite Gray) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi 9A 32Gb 2Gb (Peacook Green) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi 9A 32Gb 2Gb (Sky Blue) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi 9C 32Gb 2Gb (Sunrise Orange) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi Note 11 128GB 4Gb (Mysterious Black) CN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Xiaomi Redmi Note 11 Pro Plus 5G 128Gb 8Gb (Forest Green) </t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi Note 11E Pro 128Gb 8Gb (Atlantic Blue) CN</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi Note 11E Pro 128Gb 8Gb (Graphite Gray) CN</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi Note 11E Pro 128Gb 8Gb (Polar White) CN</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi Note 11E Pro 256Gb 8Gb (Graphite Gray) CN</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi Note 11E Pro 256Gb 8Gb (Polar White) CN</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi Note 11S 128Gb 6Gb (Graphite Gray) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi Note 11S 128Gb 6Gb (Twilight Blue) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi Pad Wi-Fi 128Gb (Moonlight Silver) CN</t>
-  </si>
-  <si>
-    <t>Xiaomi 12 Lite 5G 128Gb 8Gb (Black) RU</t>
-  </si>
-  <si>
-    <t>Xiaomi 12c 64GB 3Gb (Mint) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi 13 Lite 256Gb 8Gb (Pink) RU</t>
-  </si>
-  <si>
-    <t>Xiaomi Mix Fold 2 12Gb 256Gb (Black) CN</t>
-  </si>
-  <si>
-    <t>Xiaomi Mix Fold 2 12Gb 512Gb (Black) CN</t>
-  </si>
-  <si>
-    <t>Xiaomi Poco F4 128Gb 8Gb (Moonlight Silver) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Poco M5 128Gb 6Gb (Black) EU NFC</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi 10 128Gb 6Gb (Blue) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi 10A 128Gb 4Gb (Graphite Grey) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi 10c 64Gb 3Gb (Mint Green) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi 10c 64Gb 3Gb (Ocean Blue) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi Note 10 JE 64Gb 4Gb (White) JP</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi Note 10 Pro 128Gb 8Gb (Glacier Blue) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi Note 11 Pro 5G 64Gb 4Gb (Atlantic Blue) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi Note 11 Pro 5G 64Gb 6GB (Graphite Gray) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi Note 11 Pro Plus 5G 128Gb 8Gb (Graphite Gray) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi Note 11E Pro 256Gb 8Gb (Atlantic Blue) CN</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi Note 11R 128Gb 6GB (Black) CN</t>
+    <t>Xiaomi Redmi 10A 64Gb 3Gb (Sea Blue) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 11 Pro 5G 128Gb 8GB (Graphite Gray) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 11 Pro Plus 5G 128Gb 8Gb (Star Blue) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 11S 64Gb 6Gb (Graphite Gray) RU</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 11S 64Gb 6Gb (Twilight Blue) RU</t>
   </si>
   <si>
     <t>Xiaomi Redmi Note 12 128GB 6GB (Black) CN</t>
   </si>
   <si>
-    <t>Xiaomi Redmi Note 12 128GB 6GB (Blue) CN</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi Note 12 128GB 6GB (White) CN</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi Note 12 Pro 256GB 8GB (Black) CN</t>
+    <t>Xiaomi Redmi Note 12 128GB 6GB (Black) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 12 128GB 6GB (Frosted Green) EU</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 12 Pro 128GB 6GB (Black) EU</t>
   </si>
   <si>
     <t>Xiaomi Redmi Note 12 Pro 256GB 8GB (Blue) CN</t>
@@ -674,328 +950,7 @@
     <t>Xiaomi Redmi Note 12 Pro+ 256GB 12GB (Black) CN</t>
   </si>
   <si>
-    <t>Xiaomi Redmi Note 12 Pro+ 256GB 12GB (Blue) CN</t>
-  </si>
-  <si>
     <t>Xiaomi Redmi Note 12 Pro+ 256GB 12GB (White) CN</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi Note 12 Pro+ 256GB 8GB (Black) CN</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi Note 12 Pro+ 256GB 8GB (Blue) CN</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi Note 12 Pro+ 256GB 8GB (White) CN</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi Pad Wi-Fi 128Gb (Graphite Gray) CN</t>
-  </si>
-  <si>
-    <t>Xiaomi 12 256Gb 12GB (Blue) RU</t>
-  </si>
-  <si>
-    <t>Xiaomi 12T Pro 256Gb 8Gb (Black) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi 12c 128Gb 6GB (Gray) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi 13 Lite 256Gb 8Gb (Black) RU</t>
-  </si>
-  <si>
-    <t>Xiaomi Poco X5 Pro 256GB 8GB (Blue) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi Note 12 128GB 4Gb (Black) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi Note 12 Pro 256GB 8GB (Violet) CN</t>
-  </si>
-  <si>
-    <t>Xiaomi 12X 128Gb 8Gb (Blue) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi 12X 256Gb 8Gb (Blue) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi 12X 256Gb 8Gb (Gray) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi 12c 128Gb 6GB (Mint) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi 13 Lite 256Gb 8Gb (Black) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Poco C40 64Gb 4Gb (Poco Yellow) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Poco M5 64Gb 4Gb (Black) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Poco X3 Pro 256Gb 8Gb (Frost Blue) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Poco X4 Pro 5G 128Gb 6Gb (Laser Black) RU</t>
-  </si>
-  <si>
-    <t>Xiaomi Poco X5 128GB 6Gb (Black) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi 10 128Gb 4Gb (White) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi Note 11 Pro 128Gb 8Gb (Graphite Gray) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi Note 11 Pro 128Gb 8Gb (Polar White) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi 11T 128Gb 8Gb (Celestial Blue) RU</t>
-  </si>
-  <si>
-    <t>Xiaomi 11T 128Gb 8Gb (Meteorite Gray) RU</t>
-  </si>
-  <si>
-    <t>Xiaomi 11T 256Gb 8Gb (Meteorite Gray) RU</t>
-  </si>
-  <si>
-    <t>Xiaomi 12 Lite 5G 256Gb 8Gb (Lite Green) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi 12c 64GB 4Gb (Blue) EU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Xiaomi 13 Lite 256Gb 8Gb (Black) </t>
-  </si>
-  <si>
-    <t>Xiaomi Mi 10T 5G 128Gb 8Gb (Cosmic Black) RU</t>
-  </si>
-  <si>
-    <t>Xiaomi Mi 10T 5G 128Gb 8Gb (Lunar Silver) RU</t>
-  </si>
-  <si>
-    <t>Xiaomi Pad 5 Wi-Fi 128Gb (Cosmic Gray) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Pad 5 Wi-Fi 256Gb (Cosmic Gray) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Poco M4 Pro 4G 256Gb 8Gb (Power Black) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Poco M4 Pro 5G 64Gb 4Gb (Cool Blue) RU</t>
-  </si>
-  <si>
-    <t>Xiaomi Poco M4 Pro 5G 64Gb 4Gb (Poco Yellow) RU</t>
-  </si>
-  <si>
-    <t>Xiaomi Poco M5s 128Gb 4Gb (Blue) RU</t>
-  </si>
-  <si>
-    <t>Xiaomi Poco M5s 128Gb 4Gb (Gray) RU</t>
-  </si>
-  <si>
-    <t>Xiaomi Poco M5s 128Gb 4Gb (White) RU</t>
-  </si>
-  <si>
-    <t>Xiaomi Poco M5s 128Gb 4Gb (Yellow) RU</t>
-  </si>
-  <si>
-    <t>Xiaomi Poco X4 GT 256Gb 8Gb (Black) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Poco X4 Pro 5G 128Gb 6Gb (Laser Black) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Poco X5 Pro 128GB 6GB (Blue) RU</t>
-  </si>
-  <si>
-    <t>Xiaomi Poco X5 Pro 128GB 6GB (Yellow) RU</t>
-  </si>
-  <si>
-    <t>Xiaomi Poco X5 Pro 256GB 8GB (Yellow) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi Note 10 5G 128Gb 4Gb (Aurora Green) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi Note 10S 128Gb 8Gb (Ocean Blue) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi Note 11 128GB 4Gb (Starlight blue) CN</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi Note 11 Pro 128Gb 6Gb (Atlantic Blue) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi Note 11 Pro 5G 128Gb 6GB (Graphite Gray) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi Note 11 Pro 5G 128Gb 8GB (Graphite Gray) RU</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi Note 11S 128Gb 8Gb (Pearl White) EU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Xiaomi Redmi Note 11S 128Gb 8Gb (Twilight Blue) </t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi Note 11S 64Gb 6Gb (Pearl White) RU</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi Note 12 128GB 6GB (Frosted Green) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi 12T Pro 256Gb 12Gb (Black) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi 3 Pro (Black) CN</t>
-  </si>
-  <si>
-    <t>Xiaomi 3 Pro (White) CN</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi Note 11 Pro 128Gb 6Gb (Graphite Gray) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi Note 11 Pro 128Gb 6Gb (Polar White) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi Note 11 Pro 128Gb 6Gb (Star Blue) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi Note 11 Pro 128Gb 8Gb (Atlantic Blue) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi Note 11 Pro 128Gb 8Gb (Star Blue) RU</t>
-  </si>
-  <si>
-    <t>Xiaomi 11T Pro 128Gb 8Gb (Celestial Blue) RU</t>
-  </si>
-  <si>
-    <t>Xiaomi 11T Pro 128Gb 8Gb (Meteorite Gray) RU</t>
-  </si>
-  <si>
-    <t>Xiaomi 11T Pro 128Gb 8Gb (Moonlight White) RU</t>
-  </si>
-  <si>
-    <t>Xiaomi 12T 128Gb 8Gb (Blue) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi 12T Pro 256Gb 8Gb (Blue) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi 13 256Gb 12GB (Black) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi 13 256Gb 12GB (Flora Green) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi 13 256Gb 12GB (White) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi 13 256Gb 8GB (White) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi 13 Lite 128Gb 8Gb (Black) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi 13 Lite 128Gb 8Gb (Pink) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi 13 pro 128GB 12Gb (Ceramic Black) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Poco F4 GT 128Gb 8Gb (Knight Silver) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Poco F4 GT 256Gb 12Gb (Stealth Black) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Poco X5 128GB 6Gb (Black) RU</t>
-  </si>
-  <si>
-    <t>Xiaomi Poco X5 256Gb 8Gb (Black) RU</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi 10A 64Gb 3Gb (Sea Blue) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi Note 10 Pro 128Gb 8Gb (Onyx Gray) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi Note 10 Pro 256Gb 8Gb (Aurora Green) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi Note 11S 64Gb 6Gb (Graphite Gray) RU</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi Note 11S 64Gb 6Gb (Twilight Blue) RU</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi Note 12 Pro 256GB 8GB (White) CN</t>
-  </si>
-  <si>
-    <t>Xiaomi 12 256Gb 12GB (Gray) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi 12 Lite 5G 128Gb 6Gb (Black) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi 12c 64GB 4Gb (Gray) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Black Shark 4 Pro 256Gb 12Gb (Shadow Black) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Black Shark 5 Pro 256Gb 12Gb (Black) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Black Shark 5 Pro 256Gb 16Gb (Black) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Black Shark 5 Pro 256Gb 16Gb (White) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Mi Band 5 (Black) RU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Xiaomi Mi band 7 (Black) </t>
-  </si>
-  <si>
-    <t>Xiaomi Pad 5 Wi-Fi 128Gb (Pearl White) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Pad 5 Wi-Fi 256Gb (Pearl White) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Poco X5 Pro 256GB 8GB (Black) RU</t>
-  </si>
-  <si>
-    <t>Xiaomi Poco X5 Pro 256GB 8GB (Blue) RU</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi 10 (2022) 128gb 6gb (Carbon Grey) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi 10 64Gb 4Gb (White) EU with NFC</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi 10c 128Gb 4Gb (Ocean Blue) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi 9A 32Gb 2Gb (Aurora Green) RU/СТБ</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi Note 11 Pro 128Gb 8Gb (Graphite Gray) RU</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi Pad Wi-Fi 4Gb 128Gb (Mint Green) EU</t>
-  </si>
-  <si>
-    <t>Xiaomi Redmi Pad Wi-Fi 6Gb 128Gb (Mint Green) EU</t>
   </si>
   <si>
     <t>Заказ</t>
@@ -1411,7 +1366,7 @@
   <sheetPr codeName="Лист1">
     <outlinePr summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C324"/>
+  <dimension ref="A1:C309"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1434,57 +1389,57 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>325</v>
+        <v>310</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B2" s="6">
-        <v>21350</v>
+        <v>22050</v>
       </c>
       <c r="C2" s="11"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="8">
-        <v>21350</v>
+        <v>21650</v>
       </c>
       <c r="C3" s="12"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>243</v>
+        <v>222</v>
       </c>
       <c r="B4" s="6">
-        <v>28600</v>
+        <v>28750</v>
       </c>
       <c r="C4" s="11"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>244</v>
+        <v>223</v>
       </c>
       <c r="B5" s="8">
-        <v>28600</v>
+        <v>28500</v>
       </c>
       <c r="C5" s="12"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>245</v>
+        <v>266</v>
       </c>
       <c r="B6" s="6">
-        <v>30750</v>
+        <v>30100</v>
       </c>
       <c r="C6" s="11"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>283</v>
+        <v>4</v>
       </c>
       <c r="B7" s="8">
         <v>31200</v>
@@ -1493,1135 +1448,1135 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>284</v>
+        <v>148</v>
       </c>
       <c r="B8" s="6">
-        <v>31200</v>
+        <v>31100</v>
       </c>
       <c r="C8" s="11"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>285</v>
+        <v>204</v>
       </c>
       <c r="B9" s="8">
-        <v>31200</v>
+        <v>44650</v>
       </c>
       <c r="C9" s="12"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>4</v>
+        <v>256</v>
       </c>
       <c r="B10" s="6">
-        <v>31300</v>
+        <v>44000</v>
       </c>
       <c r="C10" s="11"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>154</v>
+        <v>290</v>
       </c>
       <c r="B11" s="8">
-        <v>31400</v>
+        <v>26650</v>
       </c>
       <c r="C11" s="12"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>223</v>
+        <v>108</v>
       </c>
       <c r="B12" s="6">
-        <v>43800</v>
+        <v>27600</v>
       </c>
       <c r="C12" s="11"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>305</v>
+        <v>5</v>
       </c>
       <c r="B13" s="8">
-        <v>43500</v>
+        <v>27800</v>
       </c>
       <c r="C13" s="12"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>306</v>
+        <v>182</v>
       </c>
       <c r="B14" s="6">
-        <v>26500</v>
+        <v>27600</v>
       </c>
       <c r="C14" s="11"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>111</v>
+        <v>149</v>
       </c>
       <c r="B15" s="8">
-        <v>26600</v>
+        <v>29050</v>
       </c>
       <c r="C15" s="12"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B16" s="6">
-        <v>27150</v>
+        <v>28750</v>
       </c>
       <c r="C16" s="11"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>193</v>
+        <v>291</v>
       </c>
       <c r="B17" s="8">
-        <v>27150</v>
+        <v>29850</v>
       </c>
       <c r="C17" s="12"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>155</v>
+        <v>292</v>
       </c>
       <c r="B18" s="6">
-        <v>28300</v>
+        <v>49950</v>
       </c>
       <c r="C18" s="11"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>19</v>
+        <v>120</v>
       </c>
       <c r="B19" s="8">
-        <v>28800</v>
+        <v>73150</v>
       </c>
       <c r="C19" s="12"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>246</v>
+        <v>109</v>
       </c>
       <c r="B20" s="6">
-        <v>29200</v>
+        <v>74050</v>
       </c>
       <c r="C20" s="11"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>148</v>
+        <v>110</v>
       </c>
       <c r="B21" s="8">
-        <v>49000</v>
+        <v>78350</v>
       </c>
       <c r="C21" s="12"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>123</v>
+        <v>248</v>
       </c>
       <c r="B22" s="6">
-        <v>71700</v>
+        <v>33800</v>
       </c>
       <c r="C22" s="11"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>112</v>
+        <v>150</v>
       </c>
       <c r="B23" s="8">
-        <v>72850</v>
+        <v>34750</v>
       </c>
       <c r="C23" s="12"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>113</v>
+        <v>293</v>
       </c>
       <c r="B24" s="6">
-        <v>76950</v>
+        <v>44650</v>
       </c>
       <c r="C24" s="11"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="B25" s="8">
-        <v>34250</v>
+        <v>51500</v>
       </c>
       <c r="C25" s="12"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>156</v>
+        <v>205</v>
       </c>
       <c r="B26" s="6">
-        <v>35600</v>
+        <v>45250</v>
       </c>
       <c r="C26" s="11"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>157</v>
+        <v>249</v>
       </c>
       <c r="B27" s="8">
-        <v>35600</v>
+        <v>43800</v>
       </c>
       <c r="C27" s="12"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>275</v>
+        <v>211</v>
       </c>
       <c r="B28" s="6">
-        <v>50100</v>
+        <v>38800</v>
       </c>
       <c r="C28" s="11"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>224</v>
+        <v>151</v>
       </c>
       <c r="B29" s="8">
-        <v>44750</v>
+        <v>38500</v>
       </c>
       <c r="C29" s="12"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>287</v>
+        <v>14</v>
       </c>
       <c r="B30" s="6">
-        <v>42550</v>
+        <v>38500</v>
       </c>
       <c r="C30" s="11"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>230</v>
+        <v>212</v>
       </c>
       <c r="B31" s="8">
-        <v>36350</v>
+        <v>40900</v>
       </c>
       <c r="C31" s="12"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>158</v>
+        <v>213</v>
       </c>
       <c r="B32" s="6">
-        <v>36350</v>
+        <v>40900</v>
       </c>
       <c r="C32" s="11"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>15</v>
+        <v>111</v>
       </c>
       <c r="B33" s="8">
-        <v>36350</v>
+        <v>39750</v>
       </c>
       <c r="C33" s="12"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>231</v>
+        <v>268</v>
       </c>
       <c r="B34" s="6">
-        <v>38550</v>
+        <v>10750</v>
       </c>
       <c r="C34" s="11"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>232</v>
+        <v>269</v>
       </c>
       <c r="B35" s="8">
-        <v>38550</v>
+        <v>10750</v>
       </c>
       <c r="C35" s="12"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>114</v>
+        <v>270</v>
       </c>
       <c r="B36" s="6">
-        <v>38550</v>
+        <v>10400</v>
       </c>
       <c r="C36" s="11"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>225</v>
+        <v>271</v>
       </c>
       <c r="B37" s="8">
-        <v>12350</v>
+        <v>10750</v>
       </c>
       <c r="C37" s="12"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>233</v>
+        <v>206</v>
       </c>
       <c r="B38" s="6">
-        <v>12350</v>
+        <v>12600</v>
       </c>
       <c r="C38" s="11"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>138</v>
+        <v>214</v>
       </c>
       <c r="B39" s="8">
-        <v>9750</v>
+        <v>12200</v>
       </c>
       <c r="C39" s="12"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B40" s="6">
-        <v>9850</v>
+        <v>9600</v>
       </c>
       <c r="C40" s="11"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>194</v>
+        <v>294</v>
       </c>
       <c r="B41" s="8">
-        <v>9850</v>
+        <v>9900</v>
       </c>
       <c r="C41" s="12"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>159</v>
+        <v>134</v>
       </c>
       <c r="B42" s="6">
-        <v>10250</v>
+        <v>8450</v>
       </c>
       <c r="C42" s="11"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>247</v>
+        <v>272</v>
       </c>
       <c r="B43" s="8">
-        <v>10250</v>
+        <v>8650</v>
       </c>
       <c r="C43" s="12"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>307</v>
+        <v>183</v>
       </c>
       <c r="B44" s="6">
-        <v>10350</v>
+        <v>9600</v>
       </c>
       <c r="C44" s="11"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B45" s="8">
-        <v>10250</v>
+        <v>10550</v>
       </c>
       <c r="C45" s="12"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>288</v>
+        <v>273</v>
       </c>
       <c r="B46" s="6">
-        <v>56950</v>
+        <v>8650</v>
       </c>
       <c r="C46" s="11"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
-        <v>289</v>
+        <v>224</v>
       </c>
       <c r="B47" s="8">
-        <v>58600</v>
+        <v>10850</v>
       </c>
       <c r="C47" s="12"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>290</v>
+        <v>153</v>
       </c>
       <c r="B48" s="6">
-        <v>56950</v>
+        <v>57100</v>
       </c>
       <c r="C48" s="11"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B49" s="8">
-        <v>54900</v>
+        <v>56000</v>
       </c>
       <c r="C49" s="12"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>162</v>
+        <v>250</v>
       </c>
       <c r="B50" s="6">
-        <v>54900</v>
+        <v>28600</v>
       </c>
       <c r="C50" s="11"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
-        <v>291</v>
+        <v>81</v>
       </c>
       <c r="B51" s="8">
-        <v>57350</v>
+        <v>29750</v>
       </c>
       <c r="C51" s="12"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>292</v>
+        <v>225</v>
       </c>
       <c r="B52" s="6">
-        <v>31150</v>
+        <v>31550</v>
       </c>
       <c r="C52" s="11"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
-        <v>83</v>
+        <v>215</v>
       </c>
       <c r="B53" s="8">
-        <v>29850</v>
+        <v>30700</v>
       </c>
       <c r="C53" s="12"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>293</v>
+        <v>207</v>
       </c>
       <c r="B54" s="6">
-        <v>31150</v>
+        <v>30400</v>
       </c>
       <c r="C54" s="11"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
-        <v>248</v>
+        <v>143</v>
       </c>
       <c r="B55" s="8">
-        <v>31500</v>
+        <v>30700</v>
       </c>
       <c r="C55" s="12"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>234</v>
+        <v>184</v>
       </c>
       <c r="B56" s="6">
-        <v>31150</v>
+        <v>32900</v>
       </c>
       <c r="C56" s="11"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
-        <v>226</v>
+        <v>155</v>
       </c>
       <c r="B57" s="8">
-        <v>30250</v>
+        <v>80950</v>
       </c>
       <c r="C57" s="12"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="B58" s="6">
-        <v>33250</v>
+        <v>79600</v>
       </c>
       <c r="C58" s="11"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
-        <v>195</v>
+        <v>257</v>
       </c>
       <c r="B59" s="8">
-        <v>33250</v>
+        <v>52850</v>
       </c>
       <c r="C59" s="12"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>294</v>
+        <v>258</v>
       </c>
       <c r="B60" s="6">
-        <v>76700</v>
+        <v>52850</v>
       </c>
       <c r="C60" s="11"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>163</v>
+        <v>226</v>
       </c>
       <c r="B61" s="8">
-        <v>78500</v>
+        <v>34550</v>
       </c>
       <c r="C61" s="12"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>164</v>
+        <v>227</v>
       </c>
       <c r="B62" s="6">
-        <v>76700</v>
+        <v>34550</v>
       </c>
       <c r="C62" s="11"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
-        <v>276</v>
+        <v>185</v>
       </c>
       <c r="B63" s="8">
-        <v>5200</v>
+        <v>121700</v>
       </c>
       <c r="C63" s="12"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>277</v>
+        <v>186</v>
       </c>
       <c r="B64" s="6">
-        <v>5200</v>
+        <v>132200</v>
       </c>
       <c r="C64" s="11"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>308</v>
+        <v>228</v>
       </c>
       <c r="B65" s="8">
-        <v>35750</v>
+        <v>29250</v>
       </c>
       <c r="C65" s="12"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>309</v>
+        <v>274</v>
       </c>
       <c r="B66" s="6">
-        <v>47550</v>
+        <v>28100</v>
       </c>
       <c r="C66" s="11"/>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
-        <v>310</v>
+        <v>259</v>
       </c>
       <c r="B67" s="8">
-        <v>52700</v>
+        <v>29450</v>
       </c>
       <c r="C67" s="12"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>311</v>
+        <v>295</v>
       </c>
       <c r="B68" s="6">
-        <v>52700</v>
+        <v>28750</v>
       </c>
       <c r="C68" s="11"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
-        <v>249</v>
+        <v>229</v>
       </c>
       <c r="B69" s="8">
-        <v>34400</v>
+        <v>29850</v>
       </c>
       <c r="C69" s="12"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>250</v>
+        <v>260</v>
       </c>
       <c r="B70" s="6">
-        <v>34400</v>
+        <v>31750</v>
       </c>
       <c r="C70" s="11"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
-        <v>312</v>
+        <v>22</v>
       </c>
       <c r="B71" s="8">
-        <v>1450</v>
+        <v>5450</v>
       </c>
       <c r="C71" s="12"/>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>313</v>
+        <v>100</v>
       </c>
       <c r="B72" s="6">
-        <v>2900</v>
+        <v>5450</v>
       </c>
       <c r="C72" s="11"/>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
-        <v>196</v>
+        <v>6</v>
       </c>
       <c r="B73" s="8">
-        <v>116000</v>
+        <v>5450</v>
       </c>
       <c r="C73" s="12"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>197</v>
+        <v>96</v>
       </c>
       <c r="B74" s="6">
-        <v>126600</v>
+        <v>7600</v>
       </c>
       <c r="C74" s="11"/>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
-        <v>251</v>
+        <v>121</v>
       </c>
       <c r="B75" s="8">
-        <v>30000</v>
+        <v>6800</v>
       </c>
       <c r="C75" s="12"/>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>314</v>
+        <v>216</v>
       </c>
       <c r="B76" s="6">
-        <v>29100</v>
+        <v>7600</v>
       </c>
       <c r="C76" s="11"/>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
-        <v>252</v>
+        <v>45</v>
       </c>
       <c r="B77" s="8">
-        <v>33100</v>
+        <v>7300</v>
       </c>
       <c r="C77" s="12"/>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>315</v>
+        <v>62</v>
       </c>
       <c r="B78" s="6">
-        <v>31200</v>
+        <v>6800</v>
       </c>
       <c r="C78" s="11"/>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="7" t="s">
-        <v>23</v>
+        <v>283</v>
       </c>
       <c r="B79" s="8">
-        <v>5500</v>
+        <v>25600</v>
       </c>
       <c r="C79" s="12"/>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>102</v>
+        <v>144</v>
       </c>
       <c r="B80" s="6">
-        <v>5500</v>
+        <v>25950</v>
       </c>
       <c r="C80" s="11"/>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
-        <v>6</v>
+        <v>145</v>
       </c>
       <c r="B81" s="8">
-        <v>5500</v>
+        <v>25950</v>
       </c>
       <c r="C81" s="12"/>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="B82" s="6">
-        <v>8650</v>
+        <v>25950</v>
       </c>
       <c r="C82" s="11"/>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
-        <v>124</v>
+        <v>187</v>
       </c>
       <c r="B83" s="8">
-        <v>7150</v>
+        <v>30800</v>
       </c>
       <c r="C83" s="12"/>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>235</v>
+        <v>37</v>
       </c>
       <c r="B84" s="6">
-        <v>7600</v>
+        <v>29250</v>
       </c>
       <c r="C84" s="11"/>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="B85" s="8">
-        <v>7150</v>
+        <v>28400</v>
       </c>
       <c r="C85" s="12"/>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>64</v>
+        <v>157</v>
       </c>
       <c r="B86" s="6">
-        <v>7250</v>
+        <v>29250</v>
       </c>
       <c r="C86" s="11"/>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="s">
-        <v>150</v>
+        <v>7</v>
       </c>
       <c r="B87" s="8">
-        <v>26000</v>
+        <v>30800</v>
       </c>
       <c r="C87" s="12"/>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
-        <v>151</v>
+        <v>251</v>
       </c>
       <c r="B88" s="6">
-        <v>25800</v>
+        <v>31650</v>
       </c>
       <c r="C88" s="11"/>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
-        <v>25</v>
+        <v>135</v>
       </c>
       <c r="B89" s="8">
-        <v>25800</v>
+        <v>30700</v>
       </c>
       <c r="C89" s="12"/>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>198</v>
+        <v>252</v>
       </c>
       <c r="B90" s="6">
-        <v>30650</v>
+        <v>40900</v>
       </c>
       <c r="C90" s="11"/>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
-        <v>39</v>
+        <v>230</v>
       </c>
       <c r="B91" s="8">
-        <v>28200</v>
+        <v>12900</v>
       </c>
       <c r="C91" s="12"/>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>26</v>
+        <v>231</v>
       </c>
       <c r="B92" s="6">
-        <v>28200</v>
+        <v>12900</v>
       </c>
       <c r="C92" s="11"/>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="7" t="s">
-        <v>165</v>
+        <v>82</v>
       </c>
       <c r="B93" s="8">
-        <v>28700</v>
+        <v>11800</v>
       </c>
       <c r="C93" s="12"/>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>7</v>
+        <v>112</v>
       </c>
       <c r="B94" s="6">
-        <v>30550</v>
+        <v>13450</v>
       </c>
       <c r="C94" s="11"/>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="7" t="s">
-        <v>295</v>
+        <v>101</v>
       </c>
       <c r="B95" s="8">
-        <v>31300</v>
+        <v>12600</v>
       </c>
       <c r="C95" s="12"/>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>140</v>
+        <v>83</v>
       </c>
       <c r="B96" s="6">
-        <v>30650</v>
+        <v>12500</v>
       </c>
       <c r="C96" s="11"/>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="7" t="s">
-        <v>296</v>
+        <v>113</v>
       </c>
       <c r="B97" s="8">
-        <v>40600</v>
+        <v>13450</v>
       </c>
       <c r="C97" s="12"/>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
-        <v>253</v>
+        <v>102</v>
       </c>
       <c r="B98" s="6">
-        <v>20100</v>
+        <v>10950</v>
       </c>
       <c r="C98" s="11"/>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="7" t="s">
-        <v>254</v>
+        <v>84</v>
       </c>
       <c r="B99" s="8">
-        <v>12750</v>
+        <v>12500</v>
       </c>
       <c r="C99" s="12"/>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>255</v>
+        <v>114</v>
       </c>
       <c r="B100" s="6">
-        <v>12750</v>
+        <v>13450</v>
       </c>
       <c r="C100" s="11"/>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="7" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="B101" s="8">
-        <v>11800</v>
+        <v>12600</v>
       </c>
       <c r="C101" s="12"/>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
-        <v>115</v>
+        <v>284</v>
       </c>
       <c r="B102" s="6">
-        <v>13250</v>
+        <v>13950</v>
       </c>
       <c r="C102" s="11"/>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="7" t="s">
-        <v>103</v>
+        <v>188</v>
       </c>
       <c r="B103" s="8">
-        <v>11300</v>
+        <v>14400</v>
       </c>
       <c r="C103" s="12"/>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
-        <v>85</v>
+        <v>31</v>
       </c>
       <c r="B104" s="6">
-        <v>11500</v>
+        <v>14400</v>
       </c>
       <c r="C104" s="11"/>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="7" t="s">
-        <v>116</v>
+        <v>217</v>
       </c>
       <c r="B105" s="8">
-        <v>13250</v>
+        <v>10300</v>
       </c>
       <c r="C105" s="12"/>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="B106" s="6">
-        <v>11300</v>
+        <v>9050</v>
       </c>
       <c r="C106" s="11"/>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B107" s="8">
-        <v>12450</v>
+        <v>9050</v>
       </c>
       <c r="C107" s="12"/>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
-        <v>117</v>
+        <v>158</v>
       </c>
       <c r="B108" s="6">
-        <v>13250</v>
+        <v>12900</v>
       </c>
       <c r="C108" s="11"/>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="7" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="B109" s="8">
-        <v>12450</v>
+        <v>9050</v>
       </c>
       <c r="C109" s="12"/>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
-        <v>199</v>
+        <v>232</v>
       </c>
       <c r="B110" s="6">
-        <v>14000</v>
+        <v>13450</v>
       </c>
       <c r="C110" s="11"/>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="7" t="s">
-        <v>32</v>
+        <v>275</v>
       </c>
       <c r="B111" s="8">
-        <v>13650</v>
+        <v>12900</v>
       </c>
       <c r="C111" s="12"/>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B112" s="6">
-        <v>10250</v>
+        <v>13450</v>
       </c>
       <c r="C112" s="11"/>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="7" t="s">
-        <v>125</v>
+        <v>234</v>
       </c>
       <c r="B113" s="8">
-        <v>9150</v>
+        <v>13450</v>
       </c>
       <c r="C113" s="12"/>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
-        <v>87</v>
+        <v>235</v>
       </c>
       <c r="B114" s="6">
-        <v>9150</v>
+        <v>13850</v>
       </c>
       <c r="C114" s="11"/>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="7" t="s">
-        <v>166</v>
+        <v>50</v>
       </c>
       <c r="B115" s="8">
-        <v>12550</v>
+        <v>15200</v>
       </c>
       <c r="C115" s="12"/>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
-        <v>88</v>
+        <v>54</v>
       </c>
       <c r="B116" s="6">
-        <v>9150</v>
+        <v>14700</v>
       </c>
       <c r="C116" s="11"/>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="7" t="s">
-        <v>256</v>
+        <v>87</v>
       </c>
       <c r="B117" s="8">
-        <v>13400</v>
+        <v>15200</v>
       </c>
       <c r="C117" s="12"/>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
-        <v>257</v>
+        <v>123</v>
       </c>
       <c r="B118" s="6">
-        <v>13400</v>
+        <v>16650</v>
       </c>
       <c r="C118" s="11"/>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="7" t="s">
-        <v>258</v>
+        <v>276</v>
       </c>
       <c r="B119" s="8">
-        <v>13400</v>
+        <v>11350</v>
       </c>
       <c r="C119" s="12"/>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
-        <v>259</v>
+        <v>277</v>
       </c>
       <c r="B120" s="6">
-        <v>13400</v>
+        <v>11350</v>
       </c>
       <c r="C120" s="11"/>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="7" t="s">
-        <v>52</v>
+        <v>278</v>
       </c>
       <c r="B121" s="8">
-        <v>14500</v>
+        <v>12300</v>
       </c>
       <c r="C121" s="12"/>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
-        <v>56</v>
+        <v>279</v>
       </c>
       <c r="B122" s="6">
-        <v>14500</v>
+        <v>11350</v>
       </c>
       <c r="C122" s="11"/>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="7" t="s">
-        <v>89</v>
+        <v>280</v>
       </c>
       <c r="B123" s="8">
-        <v>14500</v>
+        <v>26450</v>
       </c>
       <c r="C123" s="12"/>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
-        <v>126</v>
+        <v>236</v>
       </c>
       <c r="B124" s="6">
-        <v>16150</v>
+        <v>19500</v>
       </c>
       <c r="C124" s="11"/>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="7" t="s">
-        <v>237</v>
+        <v>124</v>
       </c>
       <c r="B125" s="8">
-        <v>25700</v>
+        <v>20700</v>
       </c>
       <c r="C125" s="12"/>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
-        <v>260</v>
+        <v>218</v>
       </c>
       <c r="B126" s="6">
-        <v>28300</v>
+        <v>18550</v>
       </c>
       <c r="C126" s="11"/>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="7" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="B127" s="8">
-        <v>19600</v>
+        <v>18200</v>
       </c>
       <c r="C127" s="12"/>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
-        <v>238</v>
+        <v>55</v>
       </c>
       <c r="B128" s="6">
-        <v>20600</v>
+        <v>18550</v>
       </c>
       <c r="C128" s="11"/>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="7" t="s">
-        <v>127</v>
+        <v>159</v>
       </c>
       <c r="B129" s="8">
-        <v>20600</v>
+        <v>18200</v>
       </c>
       <c r="C129" s="12"/>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
-        <v>239</v>
+        <v>95</v>
       </c>
       <c r="B130" s="6">
-        <v>18150</v>
+        <v>18650</v>
       </c>
       <c r="C130" s="11"/>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="7" t="s">
-        <v>297</v>
+        <v>56</v>
       </c>
       <c r="B131" s="8">
-        <v>18250</v>
+        <v>20100</v>
       </c>
       <c r="C131" s="12"/>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
-        <v>57</v>
+        <v>254</v>
       </c>
       <c r="B132" s="6">
-        <v>18150</v>
+        <v>20600</v>
       </c>
       <c r="C132" s="11"/>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="7" t="s">
-        <v>167</v>
+        <v>57</v>
       </c>
       <c r="B133" s="8">
-        <v>17400</v>
+        <v>19350</v>
       </c>
       <c r="C133" s="12"/>
     </row>
@@ -2630,133 +2585,133 @@
         <v>97</v>
       </c>
       <c r="B134" s="6">
-        <v>18150</v>
+        <v>19800</v>
       </c>
       <c r="C134" s="11"/>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="7" t="s">
-        <v>58</v>
+        <v>125</v>
       </c>
       <c r="B135" s="8">
-        <v>20400</v>
+        <v>20700</v>
       </c>
       <c r="C135" s="12"/>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="5" t="s">
-        <v>298</v>
+        <v>103</v>
       </c>
       <c r="B136" s="6">
-        <v>20400</v>
+        <v>20000</v>
       </c>
       <c r="C136" s="11"/>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="7" t="s">
-        <v>59</v>
+        <v>237</v>
       </c>
       <c r="B137" s="8">
-        <v>20400</v>
+        <v>23850</v>
       </c>
       <c r="C137" s="12"/>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
-        <v>99</v>
+        <v>285</v>
       </c>
       <c r="B138" s="6">
-        <v>20850</v>
+        <v>25500</v>
       </c>
       <c r="C138" s="11"/>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="7" t="s">
-        <v>128</v>
+        <v>88</v>
       </c>
       <c r="B139" s="8">
-        <v>20100</v>
+        <v>25500</v>
       </c>
       <c r="C139" s="12"/>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="5" t="s">
-        <v>105</v>
+        <v>208</v>
       </c>
       <c r="B140" s="6">
-        <v>20200</v>
+        <v>26450</v>
       </c>
       <c r="C140" s="11"/>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="7" t="s">
-        <v>262</v>
+        <v>65</v>
       </c>
       <c r="B141" s="8">
-        <v>23600</v>
+        <v>11800</v>
       </c>
       <c r="C141" s="12"/>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="5" t="s">
-        <v>263</v>
+        <v>58</v>
       </c>
       <c r="B142" s="6">
-        <v>23600</v>
+        <v>13150</v>
       </c>
       <c r="C142" s="11"/>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="7" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="B143" s="8">
-        <v>25700</v>
+        <v>12200</v>
       </c>
       <c r="C143" s="12"/>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="5" t="s">
-        <v>316</v>
+        <v>160</v>
       </c>
       <c r="B144" s="6">
-        <v>25700</v>
+        <v>13950</v>
       </c>
       <c r="C144" s="11"/>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="7" t="s">
-        <v>227</v>
+        <v>161</v>
       </c>
       <c r="B145" s="8">
-        <v>26200</v>
+        <v>12200</v>
       </c>
       <c r="C145" s="12"/>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="5" t="s">
-        <v>317</v>
+        <v>261</v>
       </c>
       <c r="B146" s="6">
-        <v>25700</v>
+        <v>14150</v>
       </c>
       <c r="C146" s="11"/>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="7" t="s">
-        <v>264</v>
+        <v>104</v>
       </c>
       <c r="B147" s="8">
-        <v>26300</v>
+        <v>13650</v>
       </c>
       <c r="C147" s="12"/>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="5" t="s">
-        <v>106</v>
+        <v>136</v>
       </c>
       <c r="B148" s="6">
-        <v>12650</v>
+        <v>12500</v>
       </c>
       <c r="C148" s="11"/>
     </row>
@@ -2765,16 +2720,16 @@
         <v>67</v>
       </c>
       <c r="B149" s="8">
-        <v>11800</v>
+        <v>9600</v>
       </c>
       <c r="C149" s="12"/>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="5" t="s">
-        <v>60</v>
+        <v>115</v>
       </c>
       <c r="B150" s="6">
-        <v>12650</v>
+        <v>12500</v>
       </c>
       <c r="C150" s="11"/>
     </row>
@@ -2783,49 +2738,49 @@
         <v>68</v>
       </c>
       <c r="B151" s="8">
-        <v>12450</v>
+        <v>9600</v>
       </c>
       <c r="C151" s="12"/>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="5" t="s">
-        <v>168</v>
+        <v>69</v>
       </c>
       <c r="B152" s="6">
-        <v>13600</v>
+        <v>9600</v>
       </c>
       <c r="C152" s="11"/>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="7" t="s">
-        <v>169</v>
+        <v>219</v>
       </c>
       <c r="B153" s="8">
-        <v>12450</v>
+        <v>12300</v>
       </c>
       <c r="C153" s="12"/>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
-        <v>318</v>
+        <v>189</v>
       </c>
       <c r="B154" s="6">
-        <v>14200</v>
+        <v>13350</v>
       </c>
       <c r="C154" s="11"/>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="7" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="B155" s="8">
-        <v>13250</v>
+        <v>13350</v>
       </c>
       <c r="C155" s="12"/>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
-        <v>141</v>
+        <v>296</v>
       </c>
       <c r="B156" s="6">
         <v>11800</v>
@@ -2834,739 +2789,739 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="7" t="s">
-        <v>69</v>
+        <v>297</v>
       </c>
       <c r="B157" s="8">
-        <v>9100</v>
+        <v>11800</v>
       </c>
       <c r="C157" s="12"/>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
-        <v>118</v>
+        <v>262</v>
       </c>
       <c r="B158" s="6">
-        <v>11800</v>
+        <v>12800</v>
       </c>
       <c r="C158" s="11"/>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="7" t="s">
-        <v>70</v>
+        <v>190</v>
       </c>
       <c r="B159" s="8">
-        <v>9100</v>
+        <v>9050</v>
       </c>
       <c r="C159" s="12"/>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="5" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="B160" s="6">
-        <v>9100</v>
+        <v>5550</v>
       </c>
       <c r="C160" s="11"/>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="7" t="s">
-        <v>240</v>
+        <v>8</v>
       </c>
       <c r="B161" s="8">
-        <v>12650</v>
+        <v>6800</v>
       </c>
       <c r="C161" s="12"/>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="5" t="s">
-        <v>200</v>
+        <v>28</v>
       </c>
       <c r="B162" s="6">
-        <v>13400</v>
+        <v>5750</v>
       </c>
       <c r="C162" s="11"/>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="7" t="s">
-        <v>33</v>
+        <v>162</v>
       </c>
       <c r="B163" s="8">
-        <v>13400</v>
+        <v>7400</v>
       </c>
       <c r="C163" s="12"/>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
-        <v>91</v>
+        <v>12</v>
       </c>
       <c r="B164" s="6">
-        <v>13400</v>
+        <v>5850</v>
       </c>
       <c r="C164" s="11"/>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="7" t="s">
-        <v>170</v>
+        <v>51</v>
       </c>
       <c r="B165" s="8">
-        <v>10350</v>
+        <v>6800</v>
       </c>
       <c r="C165" s="12"/>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
-        <v>171</v>
+        <v>19</v>
       </c>
       <c r="B166" s="6">
-        <v>10350</v>
+        <v>5550</v>
       </c>
       <c r="C166" s="11"/>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="7" t="s">
-        <v>319</v>
+        <v>33</v>
       </c>
       <c r="B167" s="8">
-        <v>12450</v>
+        <v>5550</v>
       </c>
       <c r="C167" s="12"/>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="5" t="s">
-        <v>172</v>
+        <v>34</v>
       </c>
       <c r="B168" s="6">
-        <v>10350</v>
+        <v>9050</v>
       </c>
       <c r="C168" s="11"/>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="7" t="s">
-        <v>201</v>
+        <v>38</v>
       </c>
       <c r="B169" s="8">
-        <v>9400</v>
+        <v>7950</v>
       </c>
       <c r="C169" s="12"/>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="5" t="s">
-        <v>12</v>
+        <v>298</v>
       </c>
       <c r="B170" s="6">
-        <v>5900</v>
+        <v>8150</v>
       </c>
       <c r="C170" s="11"/>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" s="7" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="B171" s="8">
-        <v>6800</v>
+        <v>9050</v>
       </c>
       <c r="C171" s="12"/>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="5" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B172" s="6">
-        <v>5700</v>
+        <v>9200</v>
       </c>
       <c r="C172" s="11"/>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="7" t="s">
-        <v>173</v>
+        <v>43</v>
       </c>
       <c r="B173" s="8">
-        <v>7150</v>
+        <v>9200</v>
       </c>
       <c r="C173" s="12"/>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="5" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="B174" s="6">
-        <v>5900</v>
+        <v>9200</v>
       </c>
       <c r="C174" s="11"/>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="7" t="s">
-        <v>53</v>
+        <v>163</v>
       </c>
       <c r="B175" s="8">
-        <v>6800</v>
+        <v>11550</v>
       </c>
       <c r="C175" s="12"/>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="5" t="s">
-        <v>20</v>
+        <v>90</v>
       </c>
       <c r="B176" s="6">
-        <v>5700</v>
+        <v>10850</v>
       </c>
       <c r="C176" s="11"/>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" s="7" t="s">
-        <v>35</v>
+        <v>164</v>
       </c>
       <c r="B177" s="8">
-        <v>6050</v>
+        <v>11550</v>
       </c>
       <c r="C177" s="12"/>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" s="5" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="B178" s="6">
-        <v>8950</v>
+        <v>10300</v>
       </c>
       <c r="C178" s="11"/>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" s="7" t="s">
-        <v>40</v>
+        <v>165</v>
       </c>
       <c r="B179" s="8">
-        <v>8100</v>
+        <v>11550</v>
       </c>
       <c r="C179" s="12"/>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" s="5" t="s">
-        <v>299</v>
+        <v>70</v>
       </c>
       <c r="B180" s="6">
-        <v>8100</v>
+        <v>10100</v>
       </c>
       <c r="C180" s="11"/>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" s="7" t="s">
-        <v>54</v>
+        <v>166</v>
       </c>
       <c r="B181" s="8">
-        <v>8950</v>
+        <v>10850</v>
       </c>
       <c r="C181" s="12"/>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" s="5" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="B182" s="6">
-        <v>8800</v>
+        <v>7950</v>
       </c>
       <c r="C182" s="11"/>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" s="7" t="s">
-        <v>45</v>
+        <v>191</v>
       </c>
       <c r="B183" s="8">
-        <v>8800</v>
+        <v>7950</v>
       </c>
       <c r="C183" s="12"/>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" s="5" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B184" s="6">
-        <v>8800</v>
+        <v>7950</v>
       </c>
       <c r="C184" s="11"/>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" s="7" t="s">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="B185" s="8">
-        <v>11200</v>
+        <v>7950</v>
       </c>
       <c r="C185" s="12"/>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" s="5" t="s">
-        <v>92</v>
+        <v>48</v>
       </c>
       <c r="B186" s="6">
-        <v>10800</v>
+        <v>7950</v>
       </c>
       <c r="C186" s="11"/>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" s="7" t="s">
-        <v>175</v>
+        <v>137</v>
       </c>
       <c r="B187" s="8">
-        <v>11200</v>
+        <v>8050</v>
       </c>
       <c r="C187" s="12"/>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" s="5" t="s">
-        <v>61</v>
+        <v>167</v>
       </c>
       <c r="B188" s="6">
-        <v>10150</v>
+        <v>10750</v>
       </c>
       <c r="C188" s="11"/>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" s="7" t="s">
-        <v>320</v>
+        <v>36</v>
       </c>
       <c r="B189" s="8">
-        <v>10700</v>
+        <v>8350</v>
       </c>
       <c r="C189" s="12"/>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" s="5" t="s">
-        <v>176</v>
+        <v>29</v>
       </c>
       <c r="B190" s="6">
-        <v>11200</v>
+        <v>8050</v>
       </c>
       <c r="C190" s="11"/>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" s="7" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="B191" s="8">
-        <v>10150</v>
+        <v>8450</v>
       </c>
       <c r="C191" s="12"/>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" s="5" t="s">
-        <v>177</v>
+        <v>26</v>
       </c>
       <c r="B192" s="6">
-        <v>10600</v>
+        <v>8050</v>
       </c>
       <c r="C192" s="11"/>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" s="7" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
       <c r="B193" s="8">
-        <v>8200</v>
+        <v>8350</v>
       </c>
       <c r="C193" s="12"/>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" s="5" t="s">
-        <v>202</v>
+        <v>71</v>
       </c>
       <c r="B194" s="6">
-        <v>8050</v>
+        <v>4700</v>
       </c>
       <c r="C194" s="11"/>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" s="7" t="s">
-        <v>37</v>
+        <v>168</v>
       </c>
       <c r="B195" s="8">
-        <v>8500</v>
+        <v>5350</v>
       </c>
       <c r="C195" s="12"/>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" s="5" t="s">
-        <v>203</v>
+        <v>63</v>
       </c>
       <c r="B196" s="6">
-        <v>8050</v>
+        <v>4600</v>
       </c>
       <c r="C196" s="11"/>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" s="7" t="s">
-        <v>50</v>
+        <v>169</v>
       </c>
       <c r="B197" s="8">
-        <v>8200</v>
+        <v>5350</v>
       </c>
       <c r="C197" s="12"/>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" s="5" t="s">
-        <v>142</v>
+        <v>98</v>
       </c>
       <c r="B198" s="6">
-        <v>8150</v>
+        <v>4600</v>
       </c>
       <c r="C198" s="11"/>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" s="7" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="B199" s="8">
-        <v>10350</v>
+        <v>5350</v>
       </c>
       <c r="C199" s="12"/>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" s="5" t="s">
-        <v>38</v>
+        <v>91</v>
       </c>
       <c r="B200" s="6">
-        <v>8300</v>
+        <v>4600</v>
       </c>
       <c r="C200" s="11"/>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" s="7" t="s">
-        <v>30</v>
+        <v>138</v>
       </c>
       <c r="B201" s="8">
-        <v>8250</v>
+        <v>10750</v>
       </c>
       <c r="C201" s="12"/>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" s="5" t="s">
-        <v>82</v>
+        <v>9</v>
       </c>
       <c r="B202" s="6">
-        <v>8300</v>
+        <v>9600</v>
       </c>
       <c r="C202" s="11"/>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" s="7" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="B203" s="8">
-        <v>8200</v>
+        <v>5950</v>
       </c>
       <c r="C203" s="12"/>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" s="5" t="s">
-        <v>21</v>
+        <v>72</v>
       </c>
       <c r="B204" s="6">
-        <v>8600</v>
+        <v>6150</v>
       </c>
       <c r="C204" s="11"/>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" s="7" t="s">
-        <v>321</v>
+        <v>171</v>
       </c>
       <c r="B205" s="8">
-        <v>4700</v>
+        <v>8250</v>
       </c>
       <c r="C205" s="12"/>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" s="5" t="s">
-        <v>73</v>
+        <v>116</v>
       </c>
       <c r="B206" s="6">
-        <v>4700</v>
+        <v>9800</v>
       </c>
       <c r="C206" s="11"/>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" s="7" t="s">
-        <v>179</v>
+        <v>117</v>
       </c>
       <c r="B207" s="8">
-        <v>5200</v>
+        <v>10950</v>
       </c>
       <c r="C207" s="12"/>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" s="5" t="s">
-        <v>65</v>
+        <v>17</v>
       </c>
       <c r="B208" s="6">
-        <v>4700</v>
+        <v>8750</v>
       </c>
       <c r="C208" s="11"/>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" s="7" t="s">
-        <v>180</v>
+        <v>64</v>
       </c>
       <c r="B209" s="8">
-        <v>5200</v>
+        <v>8650</v>
       </c>
       <c r="C209" s="12"/>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" s="5" t="s">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="B210" s="6">
-        <v>4600</v>
+        <v>7100</v>
       </c>
       <c r="C210" s="11"/>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" s="7" t="s">
-        <v>181</v>
+        <v>73</v>
       </c>
       <c r="B211" s="8">
-        <v>4800</v>
+        <v>7200</v>
       </c>
       <c r="C211" s="12"/>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" s="5" t="s">
-        <v>93</v>
+        <v>126</v>
       </c>
       <c r="B212" s="6">
-        <v>4600</v>
+        <v>8750</v>
       </c>
       <c r="C212" s="11"/>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" s="7" t="s">
-        <v>143</v>
+        <v>39</v>
       </c>
       <c r="B213" s="8">
-        <v>10250</v>
+        <v>7200</v>
       </c>
       <c r="C213" s="12"/>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" s="5" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B214" s="6">
-        <v>9650</v>
+        <v>4600</v>
       </c>
       <c r="C214" s="11"/>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" s="7" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B215" s="8">
-        <v>6050</v>
+        <v>4500</v>
       </c>
       <c r="C215" s="12"/>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" s="5" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="B216" s="6">
-        <v>6150</v>
+        <v>4600</v>
       </c>
       <c r="C216" s="11"/>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" s="7" t="s">
-        <v>182</v>
+        <v>238</v>
       </c>
       <c r="B217" s="8">
-        <v>8000</v>
+        <v>12900</v>
       </c>
       <c r="C217" s="12"/>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" s="5" t="s">
-        <v>119</v>
+        <v>193</v>
       </c>
       <c r="B218" s="6">
-        <v>9750</v>
+        <v>9300</v>
       </c>
       <c r="C218" s="11"/>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" s="7" t="s">
-        <v>120</v>
+        <v>92</v>
       </c>
       <c r="B219" s="8">
-        <v>10900</v>
+        <v>17600</v>
       </c>
       <c r="C219" s="12"/>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" s="5" t="s">
-        <v>18</v>
+        <v>105</v>
       </c>
       <c r="B220" s="6">
-        <v>8400</v>
+        <v>18200</v>
       </c>
       <c r="C220" s="11"/>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221" s="7" t="s">
-        <v>66</v>
+        <v>93</v>
       </c>
       <c r="B221" s="8">
-        <v>8600</v>
+        <v>17600</v>
       </c>
       <c r="C221" s="12"/>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" s="5" t="s">
-        <v>62</v>
+        <v>194</v>
       </c>
       <c r="B222" s="6">
-        <v>6950</v>
+        <v>19350</v>
       </c>
       <c r="C222" s="11"/>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" s="7" t="s">
-        <v>75</v>
+        <v>129</v>
       </c>
       <c r="B223" s="8">
-        <v>7150</v>
+        <v>18450</v>
       </c>
       <c r="C223" s="12"/>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" s="5" t="s">
-        <v>129</v>
+        <v>106</v>
       </c>
       <c r="B224" s="6">
-        <v>8400</v>
+        <v>13650</v>
       </c>
       <c r="C224" s="11"/>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" s="7" t="s">
-        <v>41</v>
+        <v>130</v>
       </c>
       <c r="B225" s="8">
-        <v>7150</v>
+        <v>14250</v>
       </c>
       <c r="C225" s="12"/>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" s="5" t="s">
-        <v>28</v>
+        <v>74</v>
       </c>
       <c r="B226" s="6">
-        <v>4600</v>
+        <v>13450</v>
       </c>
       <c r="C226" s="11"/>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" s="7" t="s">
-        <v>43</v>
+        <v>131</v>
       </c>
       <c r="B227" s="8">
-        <v>4500</v>
+        <v>14250</v>
       </c>
       <c r="C227" s="12"/>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228" s="5" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="B228" s="6">
-        <v>4600</v>
+        <v>13450</v>
       </c>
       <c r="C228" s="11"/>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229" s="7" t="s">
-        <v>265</v>
+        <v>132</v>
       </c>
       <c r="B229" s="8">
-        <v>12750</v>
+        <v>14250</v>
       </c>
       <c r="C229" s="12"/>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" s="5" t="s">
-        <v>204</v>
+        <v>76</v>
       </c>
       <c r="B230" s="6">
-        <v>9250</v>
+        <v>13450</v>
       </c>
       <c r="C230" s="11"/>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" s="7" t="s">
-        <v>94</v>
+        <v>286</v>
       </c>
       <c r="B231" s="8">
-        <v>17400</v>
+        <v>13350</v>
       </c>
       <c r="C231" s="12"/>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" s="5" t="s">
-        <v>108</v>
+        <v>281</v>
       </c>
       <c r="B232" s="6">
-        <v>17950</v>
+        <v>13150</v>
       </c>
       <c r="C232" s="11"/>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" s="7" t="s">
-        <v>95</v>
+        <v>287</v>
       </c>
       <c r="B233" s="8">
-        <v>17400</v>
+        <v>13350</v>
       </c>
       <c r="C233" s="12"/>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234" s="5" t="s">
-        <v>205</v>
+        <v>3</v>
       </c>
       <c r="B234" s="6">
-        <v>19300</v>
+        <v>13150</v>
       </c>
       <c r="C234" s="11"/>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" s="7" t="s">
-        <v>300</v>
+        <v>239</v>
       </c>
       <c r="B235" s="8">
-        <v>18050</v>
+        <v>15400</v>
       </c>
       <c r="C235" s="12"/>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236" s="5" t="s">
-        <v>133</v>
+        <v>172</v>
       </c>
       <c r="B236" s="6">
-        <v>17950</v>
+        <v>12200</v>
       </c>
       <c r="C236" s="11"/>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237" s="7" t="s">
-        <v>301</v>
+        <v>240</v>
       </c>
       <c r="B237" s="8">
-        <v>20000</v>
+        <v>12600</v>
       </c>
       <c r="C237" s="12"/>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238" s="5" t="s">
-        <v>134</v>
+        <v>107</v>
       </c>
       <c r="B238" s="6">
-        <v>20000</v>
+        <v>14800</v>
       </c>
       <c r="C238" s="11"/>
     </row>
@@ -3575,193 +3530,193 @@
         <v>10</v>
       </c>
       <c r="B239" s="8">
-        <v>19600</v>
+        <v>13000</v>
       </c>
       <c r="C239" s="12"/>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240" s="5" t="s">
-        <v>109</v>
+        <v>288</v>
       </c>
       <c r="B240" s="6">
-        <v>14700</v>
+        <v>13950</v>
       </c>
       <c r="C240" s="11"/>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241" s="7" t="s">
-        <v>135</v>
+        <v>289</v>
       </c>
       <c r="B241" s="8">
-        <v>14300</v>
+        <v>13950</v>
       </c>
       <c r="C241" s="12"/>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A242" s="5" t="s">
-        <v>76</v>
+        <v>139</v>
       </c>
       <c r="B242" s="6">
-        <v>13800</v>
+        <v>12900</v>
       </c>
       <c r="C242" s="11"/>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A243" s="7" t="s">
-        <v>136</v>
+        <v>77</v>
       </c>
       <c r="B243" s="8">
-        <v>14300</v>
+        <v>10550</v>
       </c>
       <c r="C243" s="12"/>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A244" s="5" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="B244" s="6">
-        <v>13800</v>
+        <v>11800</v>
       </c>
       <c r="C244" s="11"/>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A245" s="7" t="s">
-        <v>137</v>
+        <v>78</v>
       </c>
       <c r="B245" s="8">
-        <v>14300</v>
+        <v>10550</v>
       </c>
       <c r="C245" s="12"/>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A246" s="5" t="s">
-        <v>78</v>
+        <v>140</v>
       </c>
       <c r="B246" s="6">
-        <v>13800</v>
+        <v>10300</v>
       </c>
       <c r="C246" s="11"/>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247" s="7" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="B247" s="8">
-        <v>13250</v>
+        <v>11650</v>
       </c>
       <c r="C247" s="12"/>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A248" s="5" t="s">
-        <v>266</v>
+        <v>79</v>
       </c>
       <c r="B248" s="6">
-        <v>15350</v>
+        <v>10550</v>
       </c>
       <c r="C248" s="11"/>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249" s="7" t="s">
-        <v>183</v>
+        <v>241</v>
       </c>
       <c r="B249" s="8">
-        <v>11800</v>
+        <v>20300</v>
       </c>
       <c r="C249" s="12"/>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A250" s="5" t="s">
-        <v>267</v>
+        <v>245</v>
       </c>
       <c r="B250" s="6">
-        <v>12450</v>
+        <v>20400</v>
       </c>
       <c r="C250" s="11"/>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A251" s="7" t="s">
-        <v>110</v>
+        <v>246</v>
       </c>
       <c r="B251" s="8">
-        <v>14200</v>
+        <v>20400</v>
       </c>
       <c r="C251" s="12"/>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A252" s="5" t="s">
-        <v>11</v>
+        <v>247</v>
       </c>
       <c r="B252" s="6">
-        <v>12750</v>
+        <v>21750</v>
       </c>
       <c r="C252" s="11"/>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A253" s="7" t="s">
-        <v>144</v>
+        <v>220</v>
       </c>
       <c r="B253" s="8">
-        <v>12250</v>
+        <v>21350</v>
       </c>
       <c r="C253" s="12"/>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A254" s="5" t="s">
-        <v>79</v>
+        <v>263</v>
       </c>
       <c r="B254" s="6">
-        <v>10700</v>
+        <v>21950</v>
       </c>
       <c r="C254" s="11"/>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255" s="7" t="s">
-        <v>101</v>
+        <v>221</v>
       </c>
       <c r="B255" s="8">
-        <v>11800</v>
+        <v>21750</v>
       </c>
       <c r="C255" s="12"/>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A256" s="5" t="s">
-        <v>80</v>
+        <v>242</v>
       </c>
       <c r="B256" s="6">
-        <v>10350</v>
+        <v>22400</v>
       </c>
       <c r="C256" s="11"/>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A257" s="7" t="s">
-        <v>145</v>
+        <v>282</v>
       </c>
       <c r="B257" s="8">
-        <v>10350</v>
+        <v>20700</v>
       </c>
       <c r="C257" s="12"/>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A258" s="5" t="s">
-        <v>44</v>
+        <v>299</v>
       </c>
       <c r="B258" s="6">
-        <v>11800</v>
+        <v>21850</v>
       </c>
       <c r="C258" s="11"/>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A259" s="7" t="s">
-        <v>81</v>
+        <v>243</v>
       </c>
       <c r="B259" s="8">
-        <v>10150</v>
+        <v>22400</v>
       </c>
       <c r="C259" s="12"/>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A260" s="5" t="s">
-        <v>268</v>
+        <v>195</v>
       </c>
       <c r="B260" s="6">
         <v>20000</v>
@@ -3770,181 +3725,181 @@
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A261" s="7" t="s">
-        <v>278</v>
+        <v>173</v>
       </c>
       <c r="B261" s="8">
-        <v>20000</v>
+        <v>26550</v>
       </c>
       <c r="C261" s="12"/>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A262" s="5" t="s">
-        <v>279</v>
+        <v>196</v>
       </c>
       <c r="B262" s="6">
-        <v>20200</v>
+        <v>25100</v>
       </c>
       <c r="C262" s="11"/>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A263" s="7" t="s">
-        <v>280</v>
+        <v>300</v>
       </c>
       <c r="B263" s="8">
-        <v>20200</v>
+        <v>24900</v>
       </c>
       <c r="C263" s="12"/>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A264" s="5" t="s">
-        <v>281</v>
+        <v>141</v>
       </c>
       <c r="B264" s="6">
-        <v>21450</v>
+        <v>26050</v>
       </c>
       <c r="C264" s="11"/>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A265" s="7" t="s">
-        <v>241</v>
+        <v>142</v>
       </c>
       <c r="B265" s="8">
-        <v>22050</v>
+        <v>25500</v>
       </c>
       <c r="C265" s="12"/>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A266" s="5" t="s">
-        <v>322</v>
+        <v>23</v>
       </c>
       <c r="B266" s="6">
-        <v>21450</v>
+        <v>25500</v>
       </c>
       <c r="C266" s="11"/>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A267" s="7" t="s">
-        <v>242</v>
+        <v>174</v>
       </c>
       <c r="B267" s="8">
-        <v>21450</v>
+        <v>19050</v>
       </c>
       <c r="C267" s="12"/>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A268" s="5" t="s">
-        <v>282</v>
+        <v>175</v>
       </c>
       <c r="B268" s="6">
-        <v>21150</v>
+        <v>19050</v>
       </c>
       <c r="C268" s="11"/>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A269" s="7" t="s">
-        <v>269</v>
+        <v>176</v>
       </c>
       <c r="B269" s="8">
-        <v>21650</v>
+        <v>19050</v>
       </c>
       <c r="C269" s="12"/>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A270" s="5" t="s">
-        <v>270</v>
+        <v>177</v>
       </c>
       <c r="B270" s="6">
-        <v>22150</v>
+        <v>21050</v>
       </c>
       <c r="C270" s="11"/>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A271" s="7" t="s">
-        <v>206</v>
+        <v>178</v>
       </c>
       <c r="B271" s="8">
-        <v>19500</v>
+        <v>21050</v>
       </c>
       <c r="C271" s="12"/>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A272" s="5" t="s">
-        <v>207</v>
+        <v>40</v>
       </c>
       <c r="B272" s="6">
-        <v>19400</v>
+        <v>13650</v>
       </c>
       <c r="C272" s="11"/>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A273" s="7" t="s">
-        <v>184</v>
+        <v>61</v>
       </c>
       <c r="B273" s="8">
-        <v>26350</v>
+        <v>13650</v>
       </c>
       <c r="C273" s="12"/>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A274" s="5" t="s">
-        <v>208</v>
+        <v>179</v>
       </c>
       <c r="B274" s="6">
-        <v>24550</v>
+        <v>15400</v>
       </c>
       <c r="C274" s="11"/>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A275" s="7" t="s">
-        <v>146</v>
+        <v>180</v>
       </c>
       <c r="B275" s="8">
-        <v>25300</v>
+        <v>15850</v>
       </c>
       <c r="C275" s="12"/>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A276" s="5" t="s">
-        <v>147</v>
+        <v>118</v>
       </c>
       <c r="B276" s="6">
-        <v>25300</v>
+        <v>16050</v>
       </c>
       <c r="C276" s="11"/>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A277" s="7" t="s">
-        <v>24</v>
+        <v>244</v>
       </c>
       <c r="B277" s="8">
-        <v>25300</v>
+        <v>16050</v>
       </c>
       <c r="C277" s="12"/>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A278" s="5" t="s">
-        <v>185</v>
+        <v>119</v>
       </c>
       <c r="B278" s="6">
-        <v>18050</v>
+        <v>16050</v>
       </c>
       <c r="C278" s="11"/>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A279" s="7" t="s">
-        <v>186</v>
+        <v>301</v>
       </c>
       <c r="B279" s="8">
-        <v>18050</v>
+        <v>14600</v>
       </c>
       <c r="C279" s="12"/>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A280" s="5" t="s">
-        <v>187</v>
+        <v>302</v>
       </c>
       <c r="B280" s="6">
-        <v>18050</v>
+        <v>14600</v>
       </c>
       <c r="C280" s="11"/>
     </row>
@@ -3953,407 +3908,272 @@
         <v>209</v>
       </c>
       <c r="B281" s="8">
-        <v>20100</v>
+        <v>16550</v>
       </c>
       <c r="C281" s="12"/>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A282" s="5" t="s">
-        <v>188</v>
+        <v>303</v>
       </c>
       <c r="B282" s="6">
-        <v>20000</v>
+        <v>19800</v>
       </c>
       <c r="C282" s="11"/>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A283" s="7" t="s">
-        <v>189</v>
+        <v>304</v>
       </c>
       <c r="B283" s="8">
-        <v>20000</v>
+        <v>18550</v>
       </c>
       <c r="C283" s="12"/>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A284" s="5" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="B284" s="6">
-        <v>13250</v>
+        <v>18650</v>
       </c>
       <c r="C284" s="11"/>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A285" s="7" t="s">
-        <v>42</v>
+        <v>305</v>
       </c>
       <c r="B285" s="8">
-        <v>13250</v>
+        <v>18550</v>
       </c>
       <c r="C285" s="12"/>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A286" s="5" t="s">
-        <v>63</v>
+        <v>198</v>
       </c>
       <c r="B286" s="6">
-        <v>13250</v>
+        <v>18650</v>
       </c>
       <c r="C286" s="11"/>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A287" s="7" t="s">
-        <v>190</v>
+        <v>306</v>
       </c>
       <c r="B287" s="8">
-        <v>14950</v>
+        <v>25600</v>
       </c>
       <c r="C287" s="12"/>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A288" s="5" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="B288" s="6">
-        <v>15350</v>
+        <v>26550</v>
       </c>
       <c r="C288" s="11"/>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A289" s="7" t="s">
-        <v>121</v>
+        <v>307</v>
       </c>
       <c r="B289" s="8">
-        <v>15750</v>
+        <v>33950</v>
       </c>
       <c r="C289" s="12"/>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A290" s="5" t="s">
-        <v>271</v>
+        <v>210</v>
       </c>
       <c r="B290" s="6">
-        <v>15950</v>
+        <v>26550</v>
       </c>
       <c r="C290" s="11"/>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A291" s="7" t="s">
-        <v>272</v>
+        <v>255</v>
       </c>
       <c r="B291" s="8">
-        <v>15850</v>
+        <v>26550</v>
       </c>
       <c r="C291" s="12"/>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A292" s="5" t="s">
-        <v>122</v>
+        <v>308</v>
       </c>
       <c r="B292" s="6">
-        <v>15750</v>
+        <v>35050</v>
       </c>
       <c r="C292" s="11"/>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A293" s="7" t="s">
-        <v>302</v>
+        <v>200</v>
       </c>
       <c r="B293" s="8">
-        <v>14500</v>
+        <v>33400</v>
       </c>
       <c r="C293" s="12"/>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A294" s="5" t="s">
-        <v>273</v>
+        <v>309</v>
       </c>
       <c r="B294" s="6">
-        <v>14500</v>
+        <v>35050</v>
       </c>
       <c r="C294" s="11"/>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A295" s="7" t="s">
-        <v>303</v>
+        <v>201</v>
       </c>
       <c r="B295" s="8">
-        <v>14500</v>
+        <v>31950</v>
       </c>
       <c r="C295" s="12"/>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A296" s="5" t="s">
-        <v>228</v>
+        <v>202</v>
       </c>
       <c r="B296" s="6">
-        <v>16150</v>
+        <v>30300</v>
       </c>
       <c r="C296" s="11"/>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A297" s="7" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="B297" s="8">
-        <v>18550</v>
+        <v>31750</v>
       </c>
       <c r="C297" s="12"/>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A298" s="5" t="s">
-        <v>212</v>
+        <v>181</v>
       </c>
       <c r="B298" s="6">
-        <v>18450</v>
+        <v>16150</v>
       </c>
       <c r="C298" s="11"/>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A299" s="7" t="s">
-        <v>274</v>
+        <v>15</v>
       </c>
       <c r="B299" s="8">
-        <v>18050</v>
+        <v>18100</v>
       </c>
       <c r="C299" s="12"/>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A300" s="5" t="s">
-        <v>213</v>
+        <v>127</v>
       </c>
       <c r="B300" s="6">
-        <v>18450</v>
+        <v>17700</v>
       </c>
       <c r="C300" s="11"/>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A301" s="7" t="s">
-        <v>214</v>
+        <v>264</v>
       </c>
       <c r="B301" s="8">
-        <v>26300</v>
+        <v>17300</v>
       </c>
       <c r="C301" s="12"/>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A302" s="5" t="s">
-        <v>215</v>
+        <v>16</v>
       </c>
       <c r="B302" s="6">
-        <v>32850</v>
+        <v>18100</v>
       </c>
       <c r="C302" s="11"/>
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A303" s="7" t="s">
-        <v>229</v>
+        <v>128</v>
       </c>
       <c r="B303" s="8">
-        <v>26300</v>
+        <v>17700</v>
       </c>
       <c r="C303" s="12"/>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A304" s="5" t="s">
-        <v>304</v>
+        <v>30</v>
       </c>
       <c r="B304" s="6">
-        <v>26300</v>
+        <v>16150</v>
       </c>
       <c r="C304" s="11"/>
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A305" s="7" t="s">
-        <v>216</v>
+        <v>53</v>
       </c>
       <c r="B305" s="8">
-        <v>33850</v>
+        <v>16350</v>
       </c>
       <c r="C305" s="12"/>
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A306" s="5" t="s">
-        <v>217</v>
+        <v>146</v>
       </c>
       <c r="B306" s="6">
-        <v>32500</v>
+        <v>18450</v>
       </c>
       <c r="C306" s="11"/>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A307" s="7" t="s">
-        <v>218</v>
+        <v>265</v>
       </c>
       <c r="B307" s="8">
-        <v>33850</v>
+        <v>19350</v>
       </c>
       <c r="C307" s="12"/>
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A308" s="5" t="s">
-        <v>219</v>
+        <v>147</v>
       </c>
       <c r="B308" s="6">
-        <v>29650</v>
+        <v>18450</v>
       </c>
       <c r="C308" s="11"/>
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A309" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="B309" s="8">
-        <v>29650</v>
-      </c>
-      <c r="C309" s="12"/>
-    </row>
-    <row r="310" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A310" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="B310" s="6">
-        <v>29650</v>
-      </c>
-      <c r="C310" s="11"/>
-    </row>
-    <row r="311" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A311" s="7" t="s">
-        <v>222</v>
-      </c>
-      <c r="B311" s="8">
-        <v>18550</v>
-      </c>
-      <c r="C311" s="12"/>
-    </row>
-    <row r="312" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A312" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="B312" s="6">
-        <v>15350</v>
-      </c>
-      <c r="C312" s="11"/>
-    </row>
-    <row r="313" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A313" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B313" s="8">
-        <v>17900</v>
-      </c>
-      <c r="C313" s="12"/>
-    </row>
-    <row r="314" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A314" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="B314" s="6">
-        <v>17000</v>
-      </c>
-      <c r="C314" s="11"/>
-    </row>
-    <row r="315" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A315" s="7" t="s">
-        <v>323</v>
-      </c>
-      <c r="B315" s="8">
-        <v>16800</v>
-      </c>
-      <c r="C315" s="12"/>
-    </row>
-    <row r="316" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A316" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="B316" s="6">
-        <v>17500</v>
-      </c>
-      <c r="C316" s="11"/>
-    </row>
-    <row r="317" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A317" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B317" s="8">
-        <v>17900</v>
-      </c>
-      <c r="C317" s="12"/>
-    </row>
-    <row r="318" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A318" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="B318" s="6">
-        <v>17500</v>
-      </c>
-      <c r="C318" s="11"/>
-    </row>
-    <row r="319" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A319" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B319" s="8">
-        <v>15950</v>
-      </c>
-      <c r="C319" s="12"/>
-    </row>
-    <row r="320" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A320" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B320" s="6">
-        <v>16400</v>
-      </c>
-      <c r="C320" s="11"/>
-    </row>
-    <row r="321" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A321" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="B321" s="8">
-        <v>18750</v>
-      </c>
-      <c r="C321" s="12"/>
-    </row>
-    <row r="322" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A322" s="5" t="s">
-        <v>324</v>
-      </c>
-      <c r="B322" s="6">
-        <v>18750</v>
-      </c>
-      <c r="C322" s="11"/>
-    </row>
-    <row r="323" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A323" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="B323" s="8">
-        <v>18850</v>
-      </c>
-      <c r="C323" s="12"/>
-    </row>
-    <row r="324" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A324" s="9" t="s">
+      <c r="A309" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B324" s="9">
-        <f>SUMPRODUCT(B2:B323,C2:C323)</f>
+      <c r="B309" s="9">
+        <f>SUMPRODUCT(B2:B308,C2:C308)</f>
         <v>0</v>
       </c>
-      <c r="C324" s="10">
-        <f>SUM(C2:C323)</f>
+      <c r="C309" s="10">
+        <f>SUM(C2:C308)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection password="C5CB" sheet="1" objects="1" scenarios="1" autoFilter="0"/>
   <protectedRanges>
-    <protectedRange password="C5CB" sqref="A1:C324" name="Диапазон1"/>
+    <protectedRange password="C5CB" sqref="A1:C309" name="Диапазон1"/>
   </protectedRanges>
-  <autoFilter ref="A1:C324"/>
+  <autoFilter ref="A1:C309"/>
   <customSheetViews>
     <customSheetView guid="{5BF74F22-93CB-493F-8338-9D1106536A76}" showAutoFilter="1">
       <pane ySplit="1" topLeftCell="A313" activePane="bottomLeft" state="frozen"/>

</xml_diff>